<commit_message>
renumeramiento de numeros de dos DAAS y simil Puertos, COS y DAAS
</commit_message>
<xml_diff>
--- a/complete2.xlsx
+++ b/complete2.xlsx
@@ -1844,31 +1844,15 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>MEDE-CABA-H-03-DAAS</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>xe-0/0/0</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
           <t>['30', '0']</t>
         </is>
       </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>['xe-0', '0', '0']</t>
-        </is>
-      </c>
+      <c r="I32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1889,31 +1873,15 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>MEDE-CABA-H-03-DAAS</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>xe-0/0/36</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
         <is>
           <t>['30', '1']</t>
         </is>
       </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>['xe-0', '0', '36']</t>
-        </is>
-      </c>
+      <c r="I33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1934,31 +1902,15 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>MEDE-CABA-H-03-DAAS</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>xe-0/0/37</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
         <is>
           <t>['31', '0']</t>
         </is>
       </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>['xe-0', '0', '37']</t>
-        </is>
-      </c>
+      <c r="I34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1979,31 +1931,15 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>MEDE-CABA-H-03-DAAS</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>xe-0/0/38</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
         <is>
           <t>['31', '1']</t>
         </is>
       </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>['xe-0', '0', '38']</t>
-        </is>
-      </c>
+      <c r="I35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -2024,31 +1960,15 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>MEDE-CABA-H-03-DAAS</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>xe-0/0/39</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
           <t>['32', '0']</t>
         </is>
       </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>['xe-0', '0', '39']</t>
-        </is>
-      </c>
+      <c r="I36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -2069,31 +1989,15 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>MEDE-CABA-H-03-DAAS</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>xe-0/0/40</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
         <is>
           <t>['32', '1']</t>
         </is>
       </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>['xe-0', '0', '40']</t>
-        </is>
-      </c>
+      <c r="I37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -2114,31 +2018,15 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>MEDE-CABA-H-03-DAAS</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>xe-0/0/41</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr">
         <is>
           <t>['33', '0']</t>
         </is>
       </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>['xe-0', '0', '41']</t>
-        </is>
-      </c>
+      <c r="I38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -2159,31 +2047,15 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>MEDE-CABA-H-03-DAAS</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>xe-0/0/42</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr">
         <is>
           <t>['33', '1']</t>
         </is>
       </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>['xe-0', '0', '42']</t>
-        </is>
-      </c>
+      <c r="I39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -2204,31 +2076,15 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>MEDE-CABA-H-03-DAAS</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>xe-0/0/43</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
         <is>
           <t>['34', '0']</t>
         </is>
       </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>['xe-0', '0', '43']</t>
-        </is>
-      </c>
+      <c r="I40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -2249,31 +2105,15 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>MEDE-CABA-H-03-DAAS</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>xe-0/0/44</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
           <t>['34', '1']</t>
         </is>
       </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>['xe-0', '0', '44']</t>
-        </is>
-      </c>
+      <c r="I41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -2294,31 +2134,15 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>MEDE-CABA-H-03-DAAS</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>xe-0/0/45</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr">
         <is>
           <t>['35', '0']</t>
         </is>
       </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>['xe-0', '0', '45']</t>
-        </is>
-      </c>
+      <c r="I42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -2339,31 +2163,15 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>MEDE-CABA-H-03-DAAS</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>xe-0/0/46</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
         <is>
           <t>['35', '1']</t>
         </is>
       </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>['xe-0', '0', '46']</t>
-        </is>
-      </c>
+      <c r="I43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -2384,31 +2192,15 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>MEDE-CABA-H-03-DAAS</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>xe-0/0/47</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
         <is>
           <t>['36', '0']</t>
         </is>
       </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>['xe-0', '0', '47']</t>
-        </is>
-      </c>
+      <c r="I44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -2429,31 +2221,15 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>MEDE-CABA-H-03-DAAS</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>xe-0/0/48</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr">
         <is>
           <t>['36', '1']</t>
         </is>
       </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>['xe-0', '0', '48']</t>
-        </is>
-      </c>
+      <c r="I45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -2474,31 +2250,15 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>MEDE-CABA-H-03-DAAS</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>xe-0/0/5</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr">
         <is>
           <t>['37', '0']</t>
         </is>
       </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>['xe-0', '0', '5']</t>
-        </is>
-      </c>
+      <c r="I46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -2519,31 +2279,15 @@
           <t>unlocked</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>MEDE-CABA-H-03-DAAS</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>xe-0/0/7</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>PUERTOLIBRE</t>
-        </is>
-      </c>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr">
         <is>
           <t>['37', '1']</t>
         </is>
       </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>['xe-0', '0', '7']</t>
-        </is>
-      </c>
+      <c r="I47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">

</xml_diff>